<commit_message>
Actualización de script de fixtures con protección de datos
</commit_message>
<xml_diff>
--- a/Ligas/Liga_colombia_2025.xlsx
+++ b/Ligas/Liga_colombia_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D1270C-ABD1-46FE-8BE9-EFAC2B075A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF989BE-134E-46D0-B48E-F9BC23A93F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="199">
   <si>
     <t>Fecha</t>
   </si>
@@ -617,12 +617,6 @@
   </si>
   <si>
     <t>2025-06-29</t>
-  </si>
-  <si>
-    <t>Empate</t>
-  </si>
-  <si>
-    <t>Resultado</t>
   </si>
 </sst>
 </file>
@@ -685,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -693,7 +687,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S227"/>
+  <dimension ref="A1:R227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R171" sqref="R171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1016,7 @@
     <col min="18" max="18" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,11 +1071,8 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1137,11 +1127,8 @@
       <c r="R2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1196,11 +1183,8 @@
       <c r="R3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1255,11 +1239,8 @@
       <c r="R4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1314,11 +1295,8 @@
       <c r="R5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -1373,11 +1351,8 @@
       <c r="R6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1432,11 +1407,8 @@
       <c r="R7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -1491,11 +1463,8 @@
       <c r="R8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S8" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1550,11 +1519,8 @@
       <c r="R9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1609,11 +1575,8 @@
       <c r="R10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S10" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
@@ -1668,11 +1631,8 @@
       <c r="R11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S11" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1727,11 +1687,8 @@
       <c r="R12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S12" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
@@ -1786,11 +1743,8 @@
       <c r="R13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S13" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -1845,11 +1799,8 @@
       <c r="R14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S14" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1904,11 +1855,8 @@
       <c r="R15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S15" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1963,11 +1911,8 @@
       <c r="R16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S16" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2022,11 +1967,8 @@
       <c r="R17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S17" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
@@ -2081,11 +2023,8 @@
       <c r="R18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S18" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
@@ -2140,11 +2079,8 @@
       <c r="R19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S19" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -2199,11 +2135,8 @@
       <c r="R20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S20" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -2258,11 +2191,8 @@
       <c r="R21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S21" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
@@ -2317,11 +2247,8 @@
       <c r="R22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S22" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
@@ -2376,11 +2303,8 @@
       <c r="R23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S23" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -2435,11 +2359,8 @@
       <c r="R24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S24" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2494,11 +2415,8 @@
       <c r="R25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S25" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2553,11 +2471,8 @@
       <c r="R26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S26" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -2612,11 +2527,8 @@
       <c r="R27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S27" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>79</v>
       </c>
@@ -2671,11 +2583,8 @@
       <c r="R28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S28" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
@@ -2730,11 +2639,8 @@
       <c r="R29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S29" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>80</v>
       </c>
@@ -2789,11 +2695,8 @@
       <c r="R30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S30" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>81</v>
       </c>
@@ -2848,11 +2751,8 @@
       <c r="R31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S31" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>81</v>
       </c>
@@ -2907,11 +2807,8 @@
       <c r="R32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S32" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>81</v>
       </c>
@@ -2966,11 +2863,8 @@
       <c r="R33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S33" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>86</v>
       </c>
@@ -3025,11 +2919,8 @@
       <c r="R34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S34" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>86</v>
       </c>
@@ -3084,11 +2975,8 @@
       <c r="R35" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S35" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>86</v>
       </c>
@@ -3143,11 +3031,8 @@
       <c r="R36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S36" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>89</v>
       </c>
@@ -3202,11 +3087,8 @@
       <c r="R37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S37" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
@@ -3225,8 +3107,12 @@
       <c r="F38" s="2">
         <v>1336562</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="G38" s="2">
+        <v>5</v>
+      </c>
+      <c r="H38" s="2">
+        <v>4</v>
+      </c>
       <c r="I38" s="2">
         <v>3</v>
       </c>
@@ -3251,13 +3137,14 @@
       <c r="P38" s="2">
         <v>0</v>
       </c>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q38" s="2">
+        <v>55</v>
+      </c>
+      <c r="R38" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>90</v>
       </c>
@@ -3312,11 +3199,8 @@
       <c r="R39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S39" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
@@ -3371,11 +3255,8 @@
       <c r="R40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S40" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>91</v>
       </c>
@@ -3430,11 +3311,8 @@
       <c r="R41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="S41" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>94</v>
       </c>
@@ -3489,11 +3367,8 @@
       <c r="R42" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S42" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>97</v>
       </c>
@@ -3548,11 +3423,8 @@
       <c r="R43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S43" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>97</v>
       </c>
@@ -3607,11 +3479,8 @@
       <c r="R44" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="S44" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>97</v>
       </c>
@@ -3666,11 +3535,8 @@
       <c r="R45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S45" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>100</v>
       </c>
@@ -3725,11 +3591,8 @@
       <c r="R46" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S46" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>101</v>
       </c>
@@ -3784,11 +3647,8 @@
       <c r="R47" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S47" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>101</v>
       </c>
@@ -3843,11 +3703,8 @@
       <c r="R48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S48" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>102</v>
       </c>
@@ -3902,11 +3759,8 @@
       <c r="R49" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S49" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>102</v>
       </c>
@@ -3961,11 +3815,8 @@
       <c r="R50" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="S50" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>105</v>
       </c>
@@ -4020,11 +3871,8 @@
       <c r="R51" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S51" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>105</v>
       </c>
@@ -4079,11 +3927,8 @@
       <c r="R52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="S52" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -4138,11 +3983,8 @@
       <c r="R53" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S53" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>110</v>
       </c>
@@ -4197,11 +4039,8 @@
       <c r="R54" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S54" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>111</v>
       </c>
@@ -4256,11 +4095,8 @@
       <c r="R55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S55" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -4315,11 +4151,8 @@
       <c r="R56" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S56" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>113</v>
       </c>
@@ -4374,11 +4207,8 @@
       <c r="R57" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S57" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
@@ -4433,11 +4263,8 @@
       <c r="R58" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S58" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
@@ -4492,11 +4319,8 @@
       <c r="R59" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S59" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>114</v>
       </c>
@@ -4551,11 +4375,8 @@
       <c r="R60" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S60" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>115</v>
       </c>
@@ -4610,11 +4431,8 @@
       <c r="R61" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S61" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>115</v>
       </c>
@@ -4669,11 +4487,8 @@
       <c r="R62" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S62" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>115</v>
       </c>
@@ -4728,11 +4543,8 @@
       <c r="R63" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S63" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>116</v>
       </c>
@@ -4787,11 +4599,8 @@
       <c r="R64" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S64" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>117</v>
       </c>
@@ -4846,11 +4655,8 @@
       <c r="R65" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="S65" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>117</v>
       </c>
@@ -4905,11 +4711,8 @@
       <c r="R66" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S66" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>120</v>
       </c>
@@ -4964,11 +4767,8 @@
       <c r="R67" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S67" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>121</v>
       </c>
@@ -5023,11 +4823,8 @@
       <c r="R68" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S68" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>121</v>
       </c>
@@ -5082,11 +4879,8 @@
       <c r="R69" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S69" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>121</v>
       </c>
@@ -5141,11 +4935,8 @@
       <c r="R70" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S70" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>121</v>
       </c>
@@ -5200,11 +4991,8 @@
       <c r="R71" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S71" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>122</v>
       </c>
@@ -5259,11 +5047,8 @@
       <c r="R72" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="S72" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>122</v>
       </c>
@@ -5318,11 +5103,8 @@
       <c r="R73" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S73" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>122</v>
       </c>
@@ -5377,11 +5159,8 @@
       <c r="R74" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S74" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>123</v>
       </c>
@@ -5436,11 +5215,8 @@
       <c r="R75" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S75" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>123</v>
       </c>
@@ -5495,11 +5271,8 @@
       <c r="R76" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S76" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>124</v>
       </c>
@@ -5554,11 +5327,8 @@
       <c r="R77" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S77" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>125</v>
       </c>
@@ -5613,11 +5383,8 @@
       <c r="R78" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S78" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -5672,11 +5439,8 @@
       <c r="R79" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="S79" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>126</v>
       </c>
@@ -5731,11 +5495,8 @@
       <c r="R80" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S80" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>126</v>
       </c>
@@ -5790,11 +5551,8 @@
       <c r="R81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S81" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>126</v>
       </c>
@@ -5849,11 +5607,8 @@
       <c r="R82" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S82" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>127</v>
       </c>
@@ -5908,11 +5663,8 @@
       <c r="R83" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S83" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>127</v>
       </c>
@@ -5967,11 +5719,8 @@
       <c r="R84" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S84" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>127</v>
       </c>
@@ -6026,11 +5775,8 @@
       <c r="R85" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S85" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>127</v>
       </c>
@@ -6085,11 +5831,8 @@
       <c r="R86" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S86" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>128</v>
       </c>
@@ -6144,11 +5887,8 @@
       <c r="R87" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="S87" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>129</v>
       </c>
@@ -6203,11 +5943,8 @@
       <c r="R88" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S88" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>130</v>
       </c>
@@ -6262,11 +5999,8 @@
       <c r="R89" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S89" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>131</v>
       </c>
@@ -6321,11 +6055,8 @@
       <c r="R90" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="S90" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>131</v>
       </c>
@@ -6380,11 +6111,8 @@
       <c r="R91" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S91" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>131</v>
       </c>
@@ -6439,11 +6167,8 @@
       <c r="R92" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S92" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>132</v>
       </c>
@@ -6498,11 +6223,8 @@
       <c r="R93" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S93" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>132</v>
       </c>
@@ -6557,11 +6279,8 @@
       <c r="R94" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S94" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>132</v>
       </c>
@@ -6616,11 +6335,8 @@
       <c r="R95" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S95" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>133</v>
       </c>
@@ -6675,11 +6391,8 @@
       <c r="R96" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S96" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>133</v>
       </c>
@@ -6734,11 +6447,8 @@
       <c r="R97" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S97" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>133</v>
       </c>
@@ -6793,11 +6503,8 @@
       <c r="R98" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S98" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>134</v>
       </c>
@@ -6852,11 +6559,8 @@
       <c r="R99" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S99" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>134</v>
       </c>
@@ -6911,11 +6615,8 @@
       <c r="R100" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="S100" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>135</v>
       </c>
@@ -6970,11 +6671,8 @@
       <c r="R101" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S101" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>135</v>
       </c>
@@ -7029,11 +6727,8 @@
       <c r="R102" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S102" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>136</v>
       </c>
@@ -7088,11 +6783,8 @@
       <c r="R103" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S103" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>137</v>
       </c>
@@ -7147,11 +6839,8 @@
       <c r="R104" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S104" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>137</v>
       </c>
@@ -7206,11 +6895,8 @@
       <c r="R105" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="S105" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>138</v>
       </c>
@@ -7265,11 +6951,8 @@
       <c r="R106" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="S106" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>138</v>
       </c>
@@ -7324,11 +7007,8 @@
       <c r="R107" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="S107" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>138</v>
       </c>
@@ -7383,11 +7063,8 @@
       <c r="R108" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S108" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>139</v>
       </c>
@@ -7442,11 +7119,8 @@
       <c r="R109" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S109" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>140</v>
       </c>
@@ -7501,11 +7175,8 @@
       <c r="R110" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S110" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>140</v>
       </c>
@@ -7560,11 +7231,8 @@
       <c r="R111" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S111" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>141</v>
       </c>
@@ -7619,11 +7287,8 @@
       <c r="R112" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="S112" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>142</v>
       </c>
@@ -7678,11 +7343,8 @@
       <c r="R113" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="S113" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>143</v>
       </c>
@@ -7737,11 +7399,8 @@
       <c r="R114" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S114" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>143</v>
       </c>
@@ -7796,11 +7455,8 @@
       <c r="R115" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S115" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>143</v>
       </c>
@@ -7855,11 +7511,8 @@
       <c r="R116" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S116" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>143</v>
       </c>
@@ -7914,11 +7567,8 @@
       <c r="R117" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S117" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>144</v>
       </c>
@@ -7973,11 +7623,8 @@
       <c r="R118" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S118" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>144</v>
       </c>
@@ -8032,11 +7679,8 @@
       <c r="R119" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="S119" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>144</v>
       </c>
@@ -8091,11 +7735,8 @@
       <c r="R120" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S120" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>144</v>
       </c>
@@ -8150,11 +7791,8 @@
       <c r="R121" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S121" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>145</v>
       </c>
@@ -8209,11 +7847,8 @@
       <c r="R122" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S122" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>146</v>
       </c>
@@ -8268,11 +7903,8 @@
       <c r="R123" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S123" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>146</v>
       </c>
@@ -8327,11 +7959,8 @@
       <c r="R124" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S124" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>147</v>
       </c>
@@ -8386,11 +8015,8 @@
       <c r="R125" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S125" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>147</v>
       </c>
@@ -8445,11 +8071,8 @@
       <c r="R126" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S126" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>147</v>
       </c>
@@ -8504,11 +8127,8 @@
       <c r="R127" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S127" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>147</v>
       </c>
@@ -8563,11 +8183,8 @@
       <c r="R128" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S128" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>148</v>
       </c>
@@ -8622,11 +8239,8 @@
       <c r="R129" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S129" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>148</v>
       </c>
@@ -8681,11 +8295,8 @@
       <c r="R130" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S130" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8740,11 +8351,8 @@
       <c r="R131" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S131" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -8799,11 +8407,8 @@
       <c r="R132" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S132" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -8858,11 +8463,8 @@
       <c r="R133" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S133" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -8917,11 +8519,8 @@
       <c r="R134" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S134" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>151</v>
       </c>
@@ -8976,11 +8575,8 @@
       <c r="R135" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S135" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>151</v>
       </c>
@@ -9035,11 +8631,8 @@
       <c r="R136" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S136" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>151</v>
       </c>
@@ -9094,11 +8687,8 @@
       <c r="R137" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S137" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>151</v>
       </c>
@@ -9153,11 +8743,8 @@
       <c r="R138" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S138" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>152</v>
       </c>
@@ -9212,11 +8799,8 @@
       <c r="R139" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S139" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>152</v>
       </c>
@@ -9271,11 +8855,8 @@
       <c r="R140" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S140" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>153</v>
       </c>
@@ -9330,11 +8911,8 @@
       <c r="R141" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S141" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>154</v>
       </c>
@@ -9389,11 +8967,8 @@
       <c r="R142" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S142" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>154</v>
       </c>
@@ -9448,11 +9023,8 @@
       <c r="R143" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S143" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>155</v>
       </c>
@@ -9507,11 +9079,8 @@
       <c r="R144" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S144" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>155</v>
       </c>
@@ -9566,11 +9135,8 @@
       <c r="R145" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="S145" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>155</v>
       </c>
@@ -9625,11 +9191,8 @@
       <c r="R146" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S146" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>155</v>
       </c>
@@ -9684,11 +9247,8 @@
       <c r="R147" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="S147" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>156</v>
       </c>
@@ -9743,11 +9303,8 @@
       <c r="R148" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S148" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>157</v>
       </c>
@@ -9802,11 +9359,8 @@
       <c r="R149" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S149" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>158</v>
       </c>
@@ -9861,11 +9415,8 @@
       <c r="R150" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S150" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>158</v>
       </c>
@@ -9920,11 +9471,8 @@
       <c r="R151" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S151" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>158</v>
       </c>
@@ -9979,11 +9527,8 @@
       <c r="R152" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S152" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>159</v>
       </c>
@@ -10038,11 +9583,8 @@
       <c r="R153" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S153" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>159</v>
       </c>
@@ -10097,11 +9639,8 @@
       <c r="R154" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S154" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>159</v>
       </c>
@@ -10156,11 +9695,8 @@
       <c r="R155" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="S155" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>159</v>
       </c>
@@ -10215,11 +9751,8 @@
       <c r="R156" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S156" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>160</v>
       </c>
@@ -10274,11 +9807,8 @@
       <c r="R157" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S157" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>161</v>
       </c>
@@ -10333,11 +9863,8 @@
       <c r="R158" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S158" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>161</v>
       </c>
@@ -10392,11 +9919,8 @@
       <c r="R159" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S159" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>162</v>
       </c>
@@ -10451,11 +9975,8 @@
       <c r="R160" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S160" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>162</v>
       </c>
@@ -10510,11 +10031,8 @@
       <c r="R161" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S161" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>163</v>
       </c>
@@ -10569,11 +10087,8 @@
       <c r="R162" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S162" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>163</v>
       </c>
@@ -10628,11 +10143,8 @@
       <c r="R163" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S163" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
@@ -10687,11 +10199,8 @@
       <c r="R164" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S164" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
@@ -10746,11 +10255,8 @@
       <c r="R165" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S165" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>164</v>
       </c>
@@ -10805,11 +10311,8 @@
       <c r="R166" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S166" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>164</v>
       </c>
@@ -10864,11 +10367,8 @@
       <c r="R167" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S167" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>164</v>
       </c>
@@ -10923,11 +10423,8 @@
       <c r="R168" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S168" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>165</v>
       </c>
@@ -10982,11 +10479,8 @@
       <c r="R169" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S169" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>166</v>
       </c>
@@ -11041,11 +10535,8 @@
       <c r="R170" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S170" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>167</v>
       </c>
@@ -11100,11 +10591,8 @@
       <c r="R171" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="S171" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>167</v>
       </c>
@@ -11159,11 +10647,8 @@
       <c r="R172" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S172" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>168</v>
       </c>
@@ -11218,11 +10703,8 @@
       <c r="R173" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S173" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>168</v>
       </c>
@@ -11277,11 +10759,8 @@
       <c r="R174" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S174" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>168</v>
       </c>
@@ -11336,11 +10815,8 @@
       <c r="R175" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S175" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>169</v>
       </c>
@@ -11395,11 +10871,8 @@
       <c r="R176" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S176" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>169</v>
       </c>
@@ -11454,11 +10927,8 @@
       <c r="R177" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S177" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>169</v>
       </c>
@@ -11513,11 +10983,8 @@
       <c r="R178" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S178" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>170</v>
       </c>
@@ -11572,11 +11039,8 @@
       <c r="R179" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S179" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>171</v>
       </c>
@@ -11631,11 +11095,8 @@
       <c r="R180" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S180" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>172</v>
       </c>
@@ -11690,11 +11151,8 @@
       <c r="R181" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S181" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>172</v>
       </c>
@@ -11749,11 +11207,8 @@
       <c r="R182" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S182" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>173</v>
       </c>
@@ -11808,11 +11263,8 @@
       <c r="R183" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S183" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>173</v>
       </c>
@@ -11867,11 +11319,8 @@
       <c r="R184" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S184" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>173</v>
       </c>
@@ -11926,11 +11375,8 @@
       <c r="R185" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="S185" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>174</v>
       </c>
@@ -11985,11 +11431,8 @@
       <c r="R186" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S186" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>174</v>
       </c>
@@ -12044,11 +11487,8 @@
       <c r="R187" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S187" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>174</v>
       </c>
@@ -12103,11 +11543,8 @@
       <c r="R188" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S188" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>175</v>
       </c>
@@ -12162,11 +11599,8 @@
       <c r="R189" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S189" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>175</v>
       </c>
@@ -12221,11 +11655,8 @@
       <c r="R190" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S190" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>176</v>
       </c>
@@ -12280,11 +11711,8 @@
       <c r="R191" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S191" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>177</v>
       </c>
@@ -12339,11 +11767,8 @@
       <c r="R192" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S192" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>178</v>
       </c>
@@ -12398,11 +11823,8 @@
       <c r="R193" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S193" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>178</v>
       </c>
@@ -12457,11 +11879,8 @@
       <c r="R194" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S194" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>179</v>
       </c>
@@ -12516,11 +11935,8 @@
       <c r="R195" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S195" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>179</v>
       </c>
@@ -12575,11 +11991,8 @@
       <c r="R196" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="S196" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>179</v>
       </c>
@@ -12634,11 +12047,8 @@
       <c r="R197" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S197" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>179</v>
       </c>
@@ -12693,11 +12103,8 @@
       <c r="R198" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S198" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>179</v>
       </c>
@@ -12752,11 +12159,8 @@
       <c r="R199" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S199" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>179</v>
       </c>
@@ -12811,11 +12215,8 @@
       <c r="R200" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S200" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>179</v>
       </c>
@@ -12870,11 +12271,8 @@
       <c r="R201" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S201" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>180</v>
       </c>
@@ -12929,11 +12327,8 @@
       <c r="R202" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S202" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>181</v>
       </c>
@@ -12988,11 +12383,8 @@
       <c r="R203" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S203" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>181</v>
       </c>
@@ -13047,11 +12439,8 @@
       <c r="R204" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S204" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>182</v>
       </c>
@@ -13106,11 +12495,8 @@
       <c r="R205" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S205" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>183</v>
       </c>
@@ -13165,11 +12551,8 @@
       <c r="R206" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S206" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>184</v>
       </c>
@@ -13224,11 +12607,8 @@
       <c r="R207" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S207" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>184</v>
       </c>
@@ -13283,11 +12663,8 @@
       <c r="R208" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S208" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>185</v>
       </c>
@@ -13342,11 +12719,8 @@
       <c r="R209" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S209" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>186</v>
       </c>
@@ -13401,11 +12775,8 @@
       <c r="R210" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S210" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>187</v>
       </c>
@@ -13460,11 +12831,8 @@
       <c r="R211" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="S211" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>187</v>
       </c>
@@ -13519,11 +12887,8 @@
       <c r="R212" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S212" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>188</v>
       </c>
@@ -13578,11 +12943,8 @@
       <c r="R213" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="S213" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>189</v>
       </c>
@@ -13637,11 +12999,8 @@
       <c r="R214" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S214" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>190</v>
       </c>
@@ -13696,11 +13055,8 @@
       <c r="R215" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S215" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>190</v>
       </c>
@@ -13755,11 +13111,8 @@
       <c r="R216" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S216" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>191</v>
       </c>
@@ -13814,11 +13167,8 @@
       <c r="R217" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S217" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>192</v>
       </c>
@@ -13873,11 +13223,8 @@
       <c r="R218" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S218" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>193</v>
       </c>
@@ -13932,11 +13279,8 @@
       <c r="R219" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="S219" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>193</v>
       </c>
@@ -13991,11 +13335,8 @@
       <c r="R220" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S220" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>194</v>
       </c>
@@ -14050,11 +13391,8 @@
       <c r="R221" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S221" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>195</v>
       </c>
@@ -14109,11 +13447,8 @@
       <c r="R222" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S222" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>195</v>
       </c>
@@ -14168,11 +13503,8 @@
       <c r="R223" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S223" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>196</v>
       </c>
@@ -14227,11 +13559,8 @@
       <c r="R224" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S224" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>196</v>
       </c>
@@ -14286,11 +13615,8 @@
       <c r="R225" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S225" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>197</v>
       </c>
@@ -14345,11 +13671,8 @@
       <c r="R226" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S226" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>198</v>
       </c>
@@ -14403,9 +13726,6 @@
       </c>
       <c r="R227" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="S227" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar fixtures y agregar nuevas ligas
</commit_message>
<xml_diff>
--- a/Ligas/Liga_colombia_2025.xlsx
+++ b/Ligas/Liga_colombia_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S227"/>
+  <dimension ref="A1:S236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15672,6 +15672,609 @@
         </is>
       </c>
     </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>America de Cali</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>0</v>
+      </c>
+      <c r="E228" t="n">
+        <v>0</v>
+      </c>
+      <c r="F228" t="n">
+        <v>1392345</v>
+      </c>
+      <c r="G228" t="n">
+        <v>6</v>
+      </c>
+      <c r="H228" t="n">
+        <v>7</v>
+      </c>
+      <c r="I228" t="n">
+        <v>3</v>
+      </c>
+      <c r="J228" t="n">
+        <v>1</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0</v>
+      </c>
+      <c r="L228" t="n">
+        <v>0</v>
+      </c>
+      <c r="M228" t="n">
+        <v>0</v>
+      </c>
+      <c r="N228" t="n">
+        <v>0</v>
+      </c>
+      <c r="O228" t="n">
+        <v>0</v>
+      </c>
+      <c r="P228" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q228" t="n">
+        <v>41</v>
+      </c>
+      <c r="R228" t="n">
+        <v>59</v>
+      </c>
+      <c r="S228" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Once Caldas</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Atletico Nacional</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>1</v>
+      </c>
+      <c r="E229" t="n">
+        <v>3</v>
+      </c>
+      <c r="F229" t="n">
+        <v>1392346</v>
+      </c>
+      <c r="G229" t="n">
+        <v>2</v>
+      </c>
+      <c r="H229" t="n">
+        <v>7</v>
+      </c>
+      <c r="I229" t="n">
+        <v>5</v>
+      </c>
+      <c r="J229" t="n">
+        <v>2</v>
+      </c>
+      <c r="K229" t="n">
+        <v>0</v>
+      </c>
+      <c r="L229" t="n">
+        <v>0</v>
+      </c>
+      <c r="M229" t="n">
+        <v>0</v>
+      </c>
+      <c r="N229" t="n">
+        <v>0</v>
+      </c>
+      <c r="O229" t="n">
+        <v>1</v>
+      </c>
+      <c r="P229" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q229" t="n">
+        <v>39</v>
+      </c>
+      <c r="R229" t="n">
+        <v>61</v>
+      </c>
+      <c r="S229" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Deportivo Pasto</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Deportes Tolima</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>3</v>
+      </c>
+      <c r="E230" t="n">
+        <v>2</v>
+      </c>
+      <c r="F230" t="n">
+        <v>1392347</v>
+      </c>
+      <c r="G230" t="n">
+        <v>0</v>
+      </c>
+      <c r="H230" t="n">
+        <v>3</v>
+      </c>
+      <c r="I230" t="n">
+        <v>5</v>
+      </c>
+      <c r="J230" t="n">
+        <v>1</v>
+      </c>
+      <c r="K230" t="n">
+        <v>0</v>
+      </c>
+      <c r="L230" t="n">
+        <v>0</v>
+      </c>
+      <c r="M230" t="n">
+        <v>0</v>
+      </c>
+      <c r="N230" t="n">
+        <v>0</v>
+      </c>
+      <c r="O230" t="n">
+        <v>3</v>
+      </c>
+      <c r="P230" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q230" t="n">
+        <v>23</v>
+      </c>
+      <c r="R230" t="n">
+        <v>77</v>
+      </c>
+      <c r="S230" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Envigado</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Fortaleza FC</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>0</v>
+      </c>
+      <c r="E231" t="n">
+        <v>1</v>
+      </c>
+      <c r="F231" t="n">
+        <v>1392348</v>
+      </c>
+      <c r="G231" t="n">
+        <v>5</v>
+      </c>
+      <c r="H231" t="n">
+        <v>1</v>
+      </c>
+      <c r="I231" t="n">
+        <v>3</v>
+      </c>
+      <c r="J231" t="n">
+        <v>2</v>
+      </c>
+      <c r="K231" t="n">
+        <v>0</v>
+      </c>
+      <c r="L231" t="n">
+        <v>0</v>
+      </c>
+      <c r="M231" t="n">
+        <v>0</v>
+      </c>
+      <c r="N231" t="n">
+        <v>0</v>
+      </c>
+      <c r="O231" t="n">
+        <v>0</v>
+      </c>
+      <c r="P231" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q231" t="n">
+        <v>46</v>
+      </c>
+      <c r="R231" t="n">
+        <v>54</v>
+      </c>
+      <c r="S231" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2025-07-13</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Chico</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>1</v>
+      </c>
+      <c r="E232" t="n">
+        <v>1</v>
+      </c>
+      <c r="F232" t="n">
+        <v>1392349</v>
+      </c>
+      <c r="G232" t="n">
+        <v>6</v>
+      </c>
+      <c r="H232" t="n">
+        <v>4</v>
+      </c>
+      <c r="I232" t="n">
+        <v>2</v>
+      </c>
+      <c r="J232" t="n">
+        <v>2</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0</v>
+      </c>
+      <c r="L232" t="n">
+        <v>0</v>
+      </c>
+      <c r="M232" t="n">
+        <v>0</v>
+      </c>
+      <c r="N232" t="n">
+        <v>0</v>
+      </c>
+      <c r="O232" t="n">
+        <v>1</v>
+      </c>
+      <c r="P232" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q232" t="n">
+        <v>68</v>
+      </c>
+      <c r="R232" t="n">
+        <v>32</v>
+      </c>
+      <c r="S232" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2025-07-13</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Deportivo Cali</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>0</v>
+      </c>
+      <c r="E233" t="n">
+        <v>2</v>
+      </c>
+      <c r="F233" t="n">
+        <v>1392350</v>
+      </c>
+      <c r="G233" t="n">
+        <v>6</v>
+      </c>
+      <c r="H233" t="n">
+        <v>2</v>
+      </c>
+      <c r="I233" t="n">
+        <v>1</v>
+      </c>
+      <c r="J233" t="n">
+        <v>3</v>
+      </c>
+      <c r="K233" t="n">
+        <v>1</v>
+      </c>
+      <c r="L233" t="n">
+        <v>0</v>
+      </c>
+      <c r="M233" t="n">
+        <v>0</v>
+      </c>
+      <c r="N233" t="n">
+        <v>0</v>
+      </c>
+      <c r="O233" t="n">
+        <v>0</v>
+      </c>
+      <c r="P233" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q233" t="n">
+        <v>27</v>
+      </c>
+      <c r="R233" t="n">
+        <v>73</v>
+      </c>
+      <c r="S233" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2025-07-13</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Independiente Medellin</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Alianza Petrolera</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>1</v>
+      </c>
+      <c r="E234" t="n">
+        <v>1</v>
+      </c>
+      <c r="F234" t="n">
+        <v>1392351</v>
+      </c>
+      <c r="G234" t="n">
+        <v>15</v>
+      </c>
+      <c r="H234" t="n">
+        <v>3</v>
+      </c>
+      <c r="I234" t="n">
+        <v>1</v>
+      </c>
+      <c r="J234" t="n">
+        <v>2</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0</v>
+      </c>
+      <c r="L234" t="n">
+        <v>0</v>
+      </c>
+      <c r="M234" t="n">
+        <v>0</v>
+      </c>
+      <c r="N234" t="n">
+        <v>0</v>
+      </c>
+      <c r="O234" t="n">
+        <v>1</v>
+      </c>
+      <c r="P234" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q234" t="n">
+        <v>67</v>
+      </c>
+      <c r="R234" t="n">
+        <v>33</v>
+      </c>
+      <c r="S234" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2025-07-13</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Deportivo Pereira</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Santa Fe</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>2</v>
+      </c>
+      <c r="E235" t="n">
+        <v>2</v>
+      </c>
+      <c r="F235" t="n">
+        <v>1392352</v>
+      </c>
+      <c r="G235" t="n">
+        <v>7</v>
+      </c>
+      <c r="H235" t="n">
+        <v>3</v>
+      </c>
+      <c r="I235" t="n">
+        <v>3</v>
+      </c>
+      <c r="J235" t="n">
+        <v>2</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+      <c r="L235" t="n">
+        <v>1</v>
+      </c>
+      <c r="M235" t="n">
+        <v>0</v>
+      </c>
+      <c r="N235" t="n">
+        <v>0</v>
+      </c>
+      <c r="O235" t="n">
+        <v>2</v>
+      </c>
+      <c r="P235" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q235" t="n">
+        <v>69</v>
+      </c>
+      <c r="R235" t="n">
+        <v>31</v>
+      </c>
+      <c r="S235" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>La Equidad</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Rionegro Aguilas</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>0</v>
+      </c>
+      <c r="E236" t="n">
+        <v>0</v>
+      </c>
+      <c r="F236" t="n">
+        <v>1392353</v>
+      </c>
+      <c r="G236" t="n">
+        <v>2</v>
+      </c>
+      <c r="H236" t="n">
+        <v>7</v>
+      </c>
+      <c r="I236" t="n">
+        <v>2</v>
+      </c>
+      <c r="J236" t="n">
+        <v>2</v>
+      </c>
+      <c r="K236" t="n">
+        <v>1</v>
+      </c>
+      <c r="L236" t="n">
+        <v>1</v>
+      </c>
+      <c r="M236" t="n">
+        <v>0</v>
+      </c>
+      <c r="N236" t="n">
+        <v>0</v>
+      </c>
+      <c r="O236" t="n">
+        <v>0</v>
+      </c>
+      <c r="P236" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q236" t="n">
+        <v>46</v>
+      </c>
+      <c r="R236" t="n">
+        <v>54</v>
+      </c>
+      <c r="S236" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>